<commit_message>
Connector width is now smaller
</commit_message>
<xml_diff>
--- a/Projet/CSU Request/MASTER.xlsx
+++ b/Projet/CSU Request/MASTER.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Description</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>S/N</t>
+  </si>
+  <si>
+    <t>15 Decembre 2014</t>
   </si>
 </sst>
 </file>
@@ -136,7 +139,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -308,9 +311,6 @@
     <xf numFmtId="17" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -328,6 +328,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,16 +879,15 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="21" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="20" customWidth="1"/>
+    <col min="4" max="5" width="20.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="8"/>
   </cols>
@@ -945,7 +956,7 @@
       <c r="E4" s="14">
         <v>41883</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="24">
         <v>41944</v>
       </c>
     </row>
@@ -959,9 +970,13 @@
       <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
+      <c r="D5" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="4">
@@ -1021,7 +1036,7 @@
       <c r="E9" s="14">
         <v>41883</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="24">
         <v>41944</v>
       </c>
     </row>
@@ -1055,7 +1070,7 @@
       <c r="E11" s="14">
         <v>41883</v>
       </c>
-      <c r="F11" s="16"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" ht="30">
       <c r="A12" s="4">
@@ -1087,7 +1102,9 @@
       <c r="E13" s="14">
         <v>41883</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="24">
+        <v>41944</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="30">
       <c r="A14" s="4">
@@ -1119,7 +1136,9 @@
       <c r="E15" s="14">
         <v>41883</v>
       </c>
-      <c r="F15" s="16"/>
+      <c r="F15" s="24">
+        <v>41944</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="30">
       <c r="A16" s="4">
@@ -1131,9 +1150,13 @@
       <c r="C16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
+      <c r="D16" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="23"/>
     </row>
     <row r="17" spans="1:6" ht="30">
       <c r="A17" s="4">
@@ -1167,15 +1190,15 @@
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="16">
         <v>41944</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="20"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tips when mouse passing over start up step
</commit_message>
<xml_diff>
--- a/Projet/CSU Request/MASTER.xlsx
+++ b/Projet/CSU Request/MASTER.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Description</t>
   </si>
@@ -267,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,9 +319,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -879,14 +876,14 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="20" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="19" customWidth="1"/>
     <col min="4" max="5" width="20.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="8"/>
@@ -956,7 +953,7 @@
       <c r="E4" s="14">
         <v>41883</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>41944</v>
       </c>
     </row>
@@ -970,13 +967,13 @@
       <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="4">
@@ -1036,7 +1033,7 @@
       <c r="E9" s="14">
         <v>41883</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="23">
         <v>41944</v>
       </c>
     </row>
@@ -1102,7 +1099,7 @@
       <c r="E13" s="14">
         <v>41883</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="23">
         <v>41944</v>
       </c>
     </row>
@@ -1136,7 +1133,7 @@
       <c r="E15" s="14">
         <v>41883</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="23">
         <v>41944</v>
       </c>
     </row>
@@ -1150,13 +1147,13 @@
       <c r="C16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="23"/>
+      <c r="F16" s="22"/>
     </row>
     <row r="17" spans="1:6" ht="30">
       <c r="A17" s="4">
@@ -1182,8 +1179,12 @@
       <c r="C18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>24</v>
+      </c>
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="15">
@@ -1196,9 +1197,13 @@
       <c r="C19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
+      <c r="D19" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Copy Paste feature for milestone & start up steps
</commit_message>
<xml_diff>
--- a/Projet/CSU Request/MASTER.xlsx
+++ b/Projet/CSU Request/MASTER.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Description</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>15 Decembre 2014</t>
+  </si>
+  <si>
+    <t>oui, j'ai besoin d'une liste exhaustive des formes</t>
+  </si>
+  <si>
+    <t>non</t>
   </si>
 </sst>
 </file>
@@ -124,7 +130,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +149,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -267,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -336,6 +348,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -876,7 +897,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -884,7 +905,8 @@
     <col min="1" max="1" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="8" customWidth="1"/>
     <col min="3" max="3" width="70.7109375" style="19" customWidth="1"/>
-    <col min="4" max="5" width="20.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="8"/>
   </cols>
@@ -970,9 +992,7 @@
       <c r="D5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="20" t="s">
-        <v>24</v>
-      </c>
+      <c r="E5" s="24"/>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" ht="30">
@@ -985,7 +1005,9 @@
       <c r="C6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="25">
+        <v>41990</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
     </row>
@@ -999,7 +1021,9 @@
       <c r="C7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="25">
+        <v>41989</v>
+      </c>
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
     </row>
@@ -1013,7 +1037,9 @@
       <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="26" t="s">
+        <v>26</v>
+      </c>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
     </row>
@@ -1037,7 +1063,7 @@
         <v>41944</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15">
+    <row r="10" spans="1:6" ht="23.25" customHeight="1">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1079,7 +1105,9 @@
       <c r="C12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
     </row>
@@ -1150,9 +1178,7 @@
       <c r="D16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="20" t="s">
-        <v>24</v>
-      </c>
+      <c r="E16" s="24"/>
       <c r="F16" s="22"/>
     </row>
     <row r="17" spans="1:6" ht="30">
@@ -1182,9 +1208,7 @@
       <c r="D18" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>24</v>
-      </c>
+      <c r="E18" s="24"/>
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="15">
@@ -1200,9 +1224,7 @@
       <c r="D19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="20" t="s">
-        <v>24</v>
-      </c>
+      <c r="E19" s="24"/>
       <c r="F19" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add preview for step : shape + color
</commit_message>
<xml_diff>
--- a/Projet/CSU Request/MASTER.xlsx
+++ b/Projet/CSU Request/MASTER.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Mettre la description d’un step en deux lignes avec une valeur par defaut de 12 caracteres, mais qui reste néanmoins paramétrable</t>
   </si>
   <si>
-    <t>Serait-il possible de diversifier encore plus les formes des steps ? par exemple des étoiles, etc …</t>
-  </si>
-  <si>
     <t>Lorsque l’on ferme un projet, on ferme également le logiciel. serait il possible de dissocier les deux ?</t>
   </si>
   <si>
@@ -97,13 +94,25 @@
   </si>
   <si>
     <t>non</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Handle when ss table got null for sus field</t>
+  </si>
+  <si>
+    <t>BUG Print liste des ss pour une milestone</t>
+  </si>
+  <si>
+    <t>Serait-il possible de diversifier encore plus les formes des steps ? par exemple des étoiles, etc … + ajout d'un preview</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +137,11 @@
       <color rgb="FF92D050"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -279,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -357,6 +371,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -595,8 +627,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F21"/>
   <tableColumns count="6">
     <tableColumn id="1" name="S/N" dataDxfId="5"/>
     <tableColumn id="2" name="Submitted Date" dataDxfId="4"/>
@@ -894,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -913,22 +945,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15">
@@ -990,7 +1022,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="24"/>
       <c r="F5" s="21"/>
@@ -1019,7 +1051,7 @@
         <v>41883</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="25">
         <v>41989</v>
@@ -1038,7 +1070,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
@@ -1103,10 +1135,10 @@
         <v>41883</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
@@ -1119,7 +1151,7 @@
         <v>41883</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="14">
         <v>41883</v>
@@ -1139,7 +1171,7 @@
         <v>41883</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -1153,7 +1185,7 @@
         <v>41883</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="14">
         <v>41883</v>
@@ -1173,10 +1205,10 @@
         <v>41883</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="22"/>
@@ -1189,7 +1221,7 @@
         <v>41883</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -1203,10 +1235,10 @@
         <v>41883</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="11"/>
@@ -1219,13 +1251,49 @@
         <v>41944</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:6" ht="15">
+      <c r="A20" s="27">
+        <v>19</v>
+      </c>
+      <c r="B20" s="28">
+        <v>41913</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15">
+      <c r="A21" s="27">
+        <v>20</v>
+      </c>
+      <c r="B21" s="28">
+        <v>41913</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cancelling of NULL case for milestone field in ICAPS Db
</commit_message>
<xml_diff>
--- a/Projet/CSU Request/MASTER.xlsx
+++ b/Projet/CSU Request/MASTER.xlsx
@@ -293,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -389,6 +389,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -929,7 +932,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -1287,7 +1290,9 @@
       <c r="C21" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="30"/>
+      <c r="D21" s="33">
+        <v>42010</v>
+      </c>
       <c r="E21" s="31" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
BUG FIX : Copy Paste milestone & Steps
</commit_message>
<xml_diff>
--- a/Projet/CSU Request/MASTER.xlsx
+++ b/Projet/CSU Request/MASTER.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Description</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>oui, j'ai besoin d'une liste exhaustive des formes + 1/2</t>
+  </si>
+  <si>
+    <t>The milestone field has to be filled with String at least "N/A" for example</t>
   </si>
 </sst>
 </file>
@@ -293,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,9 +367,6 @@
     <xf numFmtId="17" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -382,9 +382,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -392,6 +389,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -932,7 +932,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -1027,7 +1027,9 @@
       <c r="D5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="24">
+        <v>42010</v>
+      </c>
       <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" ht="30">
@@ -1040,10 +1042,12 @@
       <c r="C6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>41990</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="24">
+        <v>42010</v>
+      </c>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="45">
@@ -1056,10 +1060,12 @@
       <c r="C7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>41989</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="24">
+        <v>42010</v>
+      </c>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" ht="15">
@@ -1072,7 +1078,7 @@
       <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="25" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="10"/>
@@ -1140,7 +1146,7 @@
       <c r="C12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="25" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="10"/>
@@ -1213,7 +1219,9 @@
       <c r="D16" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="24"/>
+      <c r="E16" s="24">
+        <v>42010</v>
+      </c>
       <c r="F16" s="22"/>
     </row>
     <row r="17" spans="1:6" ht="30">
@@ -1243,7 +1251,9 @@
       <c r="D18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="24"/>
+      <c r="E18" s="24">
+        <v>42010</v>
+      </c>
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="15">
@@ -1259,44 +1269,48 @@
       <c r="D19" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="24"/>
+      <c r="E19" s="24">
+        <v>42010</v>
+      </c>
       <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6" ht="15">
-      <c r="A20" s="27">
+      <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="27">
         <v>41913</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="31" t="s">
+      <c r="D20" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="32" t="s">
+      <c r="F20" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15">
-      <c r="A21" s="27">
+      <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="27">
         <v>41913</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="31">
         <v>42010</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="30" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>